<commit_message>
create Enity and first run
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C9496-80DF-47A4-ADDE-75F003226DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AD2C64-0112-4E43-966D-D656530094D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Phân quyền </t>
   </si>
   <si>
-    <t>Quản lý kho</t>
-  </si>
-  <si>
     <t>Quản lý bán hàng</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Thống kê</t>
+  </si>
+  <si>
+    <t>Quản lý sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -476,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -532,7 +532,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -546,7 +546,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>

</xml_diff>